<commit_message>
Updated pair correlation script to enable arbitrary start and ened dates.
</commit_message>
<xml_diff>
--- a/PairCorrelation/Asset1Data.xlsx
+++ b/PairCorrelation/Asset1Data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E190"/>
+  <dimension ref="A1:E183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,16 +466,16 @@
         <v>44927</v>
       </c>
       <c r="B2" t="n">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C2" t="n">
-        <v>5.226208554793322</v>
+        <v>1196.61306480845</v>
       </c>
       <c r="D2" t="n">
-        <v>201180223.6842441</v>
+        <v>144188788703.9747</v>
       </c>
       <c r="E2" t="n">
-        <v>2626588.270427597</v>
+        <v>2891351007.425189</v>
       </c>
     </row>
     <row r="3">
@@ -483,16 +483,16 @@
         <v>44928</v>
       </c>
       <c r="B3" t="n">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C3" t="n">
-        <v>5.292436808462408</v>
+        <v>1200.65921690107</v>
       </c>
       <c r="D3" t="n">
-        <v>203391756.7805569</v>
+        <v>144712215098.1516</v>
       </c>
       <c r="E3" t="n">
-        <v>4413106.49510162</v>
+        <v>2179799161.038537</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         <v>44929</v>
       </c>
       <c r="B4" t="n">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C4" t="n">
-        <v>5.32056438397027</v>
+        <v>1214.378945925351</v>
       </c>
       <c r="D4" t="n">
-        <v>204867574.3231745</v>
+        <v>146443084804.9009</v>
       </c>
       <c r="E4" t="n">
-        <v>3170460.618115874</v>
+        <v>3845095582.093461</v>
       </c>
     </row>
     <row r="5">
@@ -517,16 +517,16 @@
         <v>44930</v>
       </c>
       <c r="B5" t="n">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C5" t="n">
-        <v>5.46382760817556</v>
+        <v>1214.760969419338</v>
       </c>
       <c r="D5" t="n">
-        <v>210252238.8686023</v>
+        <v>146422424046.4976</v>
       </c>
       <c r="E5" t="n">
-        <v>3974491.679909794</v>
+        <v>3385566691.456905</v>
       </c>
     </row>
     <row r="6">
@@ -534,16 +534,16 @@
         <v>44931</v>
       </c>
       <c r="B6" t="n">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C6" t="n">
-        <v>5.383470851366112</v>
+        <v>1256.436603783486</v>
       </c>
       <c r="D6" t="n">
-        <v>207562882.8285181</v>
+        <v>151322902029.0838</v>
       </c>
       <c r="E6" t="n">
-        <v>3644370.029693644</v>
+        <v>6727208484.546551</v>
       </c>
     </row>
     <row r="7">
@@ -551,16 +551,16 @@
         <v>44932</v>
       </c>
       <c r="B7" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C7" t="n">
-        <v>5.41893704489887</v>
+        <v>1250.792252235591</v>
       </c>
       <c r="D7" t="n">
-        <v>209072307.5603918</v>
+        <v>150805231900.3949</v>
       </c>
       <c r="E7" t="n">
-        <v>4121282.677144946</v>
+        <v>4052351544.820186</v>
       </c>
     </row>
     <row r="8">
@@ -568,16 +568,16 @@
         <v>44933</v>
       </c>
       <c r="B8" t="n">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C8" t="n">
-        <v>5.344888086204569</v>
+        <v>1270.028610178057</v>
       </c>
       <c r="D8" t="n">
-        <v>206201625.705999</v>
+        <v>153115414332.1746</v>
       </c>
       <c r="E8" t="n">
-        <v>2949283.32276946</v>
+        <v>5222706873.557585</v>
       </c>
     </row>
     <row r="9">
@@ -585,16 +585,16 @@
         <v>44934</v>
       </c>
       <c r="B9" t="n">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C9" t="n">
-        <v>5.550962226602027</v>
+        <v>1264.83694338372</v>
       </c>
       <c r="D9" t="n">
-        <v>214348717.8299726</v>
+        <v>152351777734.9695</v>
       </c>
       <c r="E9" t="n">
-        <v>3468701.137509333</v>
+        <v>2439388823.057228</v>
       </c>
     </row>
     <row r="10">
@@ -602,16 +602,16 @@
         <v>44935</v>
       </c>
       <c r="B10" t="n">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C10" t="n">
-        <v>5.560195014250711</v>
+        <v>1284.575404134299</v>
       </c>
       <c r="D10" t="n">
-        <v>215052705.2206658</v>
+        <v>154857941332.0086</v>
       </c>
       <c r="E10" t="n">
-        <v>6538732.997585454</v>
+        <v>3401917835.269408</v>
       </c>
     </row>
     <row r="11">
@@ -619,16 +619,16 @@
         <v>44936</v>
       </c>
       <c r="B11" t="n">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C11" t="n">
-        <v>5.669186454865426</v>
+        <v>1321.676571173056</v>
       </c>
       <c r="D11" t="n">
-        <v>218769028.3237775</v>
+        <v>159397504473.2767</v>
       </c>
       <c r="E11" t="n">
-        <v>5497164.190982978</v>
+        <v>8615288094.160769</v>
       </c>
     </row>
     <row r="12">
@@ -636,16 +636,16 @@
         <v>44937</v>
       </c>
       <c r="B12" t="n">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C12" t="n">
-        <v>5.858650358599266</v>
+        <v>1336.017071771777</v>
       </c>
       <c r="D12" t="n">
-        <v>226342609.6782421</v>
+        <v>160999220384.6191</v>
       </c>
       <c r="E12" t="n">
-        <v>7214790.390786652</v>
+        <v>6390063040.044838</v>
       </c>
     </row>
     <row r="13">
@@ -653,16 +653,16 @@
         <v>44938</v>
       </c>
       <c r="B13" t="n">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C13" t="n">
-        <v>6.089703977852935</v>
+        <v>1389.771662094107</v>
       </c>
       <c r="D13" t="n">
-        <v>235703240.7650284</v>
+        <v>167839113151.0311</v>
       </c>
       <c r="E13" t="n">
-        <v>8639832.108701129</v>
+        <v>6779329581.863201</v>
       </c>
     </row>
     <row r="14">
@@ -670,16 +670,16 @@
         <v>44939</v>
       </c>
       <c r="B14" t="n">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C14" t="n">
-        <v>6.194581639530733</v>
+        <v>1417.134908743914</v>
       </c>
       <c r="D14" t="n">
-        <v>239541965.3364263</v>
+        <v>170890542806.2607</v>
       </c>
       <c r="E14" t="n">
-        <v>5916690.495849176</v>
+        <v>13360962683.07227</v>
       </c>
     </row>
     <row r="15">
@@ -687,16 +687,16 @@
         <v>44940</v>
       </c>
       <c r="B15" t="n">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C15" t="n">
-        <v>6.580658285348739</v>
+        <v>1453.376910208922</v>
       </c>
       <c r="D15" t="n">
-        <v>255150626.0920531</v>
+        <v>174798760594.5878</v>
       </c>
       <c r="E15" t="n">
-        <v>17400942.07157798</v>
+        <v>8386970426.225097</v>
       </c>
     </row>
     <row r="16">
@@ -704,16 +704,16 @@
         <v>44941</v>
       </c>
       <c r="B16" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C16" t="n">
-        <v>6.585765863970431</v>
+        <v>1549.111474081304</v>
       </c>
       <c r="D16" t="n">
-        <v>255154019.2319745</v>
+        <v>187276048380.949</v>
       </c>
       <c r="E16" t="n">
-        <v>7419408.355352408</v>
+        <v>15505376250.71231</v>
       </c>
     </row>
     <row r="17">
@@ -721,16 +721,16 @@
         <v>44942</v>
       </c>
       <c r="B17" t="n">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C17" t="n">
-        <v>6.734407135279036</v>
+        <v>1551.324517175301</v>
       </c>
       <c r="D17" t="n">
-        <v>261652513.2218203</v>
+        <v>186901700956.4831</v>
       </c>
       <c r="E17" t="n">
-        <v>7536570.791717867</v>
+        <v>7074931051.083694</v>
       </c>
     </row>
     <row r="18">
@@ -738,16 +738,16 @@
         <v>44943</v>
       </c>
       <c r="B18" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C18" t="n">
-        <v>6.682224445874841</v>
+        <v>1577.725890482971</v>
       </c>
       <c r="D18" t="n">
-        <v>259121681.419645</v>
+        <v>190122961411.6948</v>
       </c>
       <c r="E18" t="n">
-        <v>5918430.038917508</v>
+        <v>9434570734.551754</v>
       </c>
     </row>
     <row r="19">
@@ -755,16 +755,16 @@
         <v>44944</v>
       </c>
       <c r="B19" t="n">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C19" t="n">
-        <v>6.341895862657537</v>
+        <v>1569.530833227292</v>
       </c>
       <c r="D19" t="n">
-        <v>246710631.056621</v>
+        <v>188982728685.0974</v>
       </c>
       <c r="E19" t="n">
-        <v>8893563.171570059</v>
+        <v>8482482040.670269</v>
       </c>
     </row>
     <row r="20">
@@ -772,16 +772,16 @@
         <v>44945</v>
       </c>
       <c r="B20" t="n">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C20" t="n">
-        <v>6.571475061096788</v>
+        <v>1516.555475473704</v>
       </c>
       <c r="D20" t="n">
-        <v>255885564.8149788</v>
+        <v>183517931282.5893</v>
       </c>
       <c r="E20" t="n">
-        <v>5001701.509263325</v>
+        <v>11809477723.65587</v>
       </c>
     </row>
     <row r="21">
@@ -789,16 +789,16 @@
         <v>44946</v>
       </c>
       <c r="B21" t="n">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C21" t="n">
-        <v>7.05313652277976</v>
+        <v>1550.508887558564</v>
       </c>
       <c r="D21" t="n">
-        <v>273420374.025501</v>
+        <v>186967330908.3236</v>
       </c>
       <c r="E21" t="n">
-        <v>6413498.063327346</v>
+        <v>6871702648.394773</v>
       </c>
     </row>
     <row r="22">
@@ -806,16 +806,16 @@
         <v>44947</v>
       </c>
       <c r="B22" t="n">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C22" t="n">
-        <v>6.840494770918017</v>
+        <v>1661.33491934054</v>
       </c>
       <c r="D22" t="n">
-        <v>265797245.8049646</v>
+        <v>200011161010.5197</v>
       </c>
       <c r="E22" t="n">
-        <v>7848673.945877104</v>
+        <v>9228892411.460192</v>
       </c>
     </row>
     <row r="23">
@@ -823,16 +823,16 @@
         <v>44948</v>
       </c>
       <c r="B23" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C23" t="n">
-        <v>6.842611806030692</v>
+        <v>1625.909310988656</v>
       </c>
       <c r="D23" t="n">
-        <v>266178986.4506937</v>
+        <v>195908718395.0808</v>
       </c>
       <c r="E23" t="n">
-        <v>6058062.593590341</v>
+        <v>9663018503.707115</v>
       </c>
     </row>
     <row r="24">
@@ -840,16 +840,16 @@
         <v>44949</v>
       </c>
       <c r="B24" t="n">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C24" t="n">
-        <v>6.938496063243634</v>
+        <v>1630.844854940797</v>
       </c>
       <c r="D24" t="n">
-        <v>269743914.1258465</v>
+        <v>196512572594.4076</v>
       </c>
       <c r="E24" t="n">
-        <v>8782153.387244968</v>
+        <v>8233555835.053316</v>
       </c>
     </row>
     <row r="25">
@@ -857,16 +857,16 @@
         <v>44950</v>
       </c>
       <c r="B25" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C25" t="n">
-        <v>6.695674913280592</v>
+        <v>1632.961726713527</v>
       </c>
       <c r="D25" t="n">
-        <v>260164130.5039959</v>
+        <v>196541663696.4374</v>
       </c>
       <c r="E25" t="n">
-        <v>10664130.86553231</v>
+        <v>9037743837.862547</v>
       </c>
     </row>
     <row r="26">
@@ -874,16 +874,16 @@
         <v>44951</v>
       </c>
       <c r="B26" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C26" t="n">
-        <v>6.939699313625209</v>
+        <v>1557.059760872173</v>
       </c>
       <c r="D26" t="n">
-        <v>269748934.8782283</v>
+        <v>187270576772.9432</v>
       </c>
       <c r="E26" t="n">
-        <v>11857049.97085386</v>
+        <v>9078639809.982983</v>
       </c>
     </row>
     <row r="27">
@@ -891,16 +891,16 @@
         <v>44952</v>
       </c>
       <c r="B27" t="n">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C27" t="n">
-        <v>6.896129021827281</v>
+        <v>1614.67718506293</v>
       </c>
       <c r="D27" t="n">
-        <v>269049142.1101401</v>
+        <v>194402223992.6201</v>
       </c>
       <c r="E27" t="n">
-        <v>9599613.291887918</v>
+        <v>11946053798.49039</v>
       </c>
     </row>
     <row r="28">
@@ -908,16 +908,16 @@
         <v>44953</v>
       </c>
       <c r="B28" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C28" t="n">
-        <v>6.908529487413467</v>
+        <v>1602.846949252319</v>
       </c>
       <c r="D28" t="n">
-        <v>269639532.3489422</v>
+        <v>193276131177.5974</v>
       </c>
       <c r="E28" t="n">
-        <v>8717630.898924796</v>
+        <v>10076436860.256</v>
       </c>
     </row>
     <row r="29">
@@ -925,16 +925,16 @@
         <v>44954</v>
       </c>
       <c r="B29" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C29" t="n">
-        <v>6.824232757805255</v>
+        <v>1598.470193545005</v>
       </c>
       <c r="D29" t="n">
-        <v>266516042.7900164</v>
+        <v>192677648328.4367</v>
       </c>
       <c r="E29" t="n">
-        <v>17168029.06885294</v>
+        <v>9593062923.130283</v>
       </c>
     </row>
     <row r="30">
@@ -942,16 +942,16 @@
         <v>44955</v>
       </c>
       <c r="B30" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C30" t="n">
-        <v>7.138990469309625</v>
+        <v>1573.063439433065</v>
       </c>
       <c r="D30" t="n">
-        <v>278492703.9045178</v>
+        <v>189301295262.2017</v>
       </c>
       <c r="E30" t="n">
-        <v>9079700.118441137</v>
+        <v>6523949724.808857</v>
       </c>
     </row>
     <row r="31">
@@ -959,16 +959,16 @@
         <v>44956</v>
       </c>
       <c r="B31" t="n">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C31" t="n">
-        <v>6.637023118143855</v>
+        <v>1646.51599009302</v>
       </c>
       <c r="D31" t="n">
-        <v>259082302.6170296</v>
+        <v>198339307428.1037</v>
       </c>
       <c r="E31" t="n">
-        <v>13792000.7203127</v>
+        <v>10037370816.30801</v>
       </c>
     </row>
     <row r="32">
@@ -976,16 +976,16 @@
         <v>44957</v>
       </c>
       <c r="B32" t="n">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C32" t="n">
-        <v>6.682340093865529</v>
+        <v>1568.64771349631</v>
       </c>
       <c r="D32" t="n">
-        <v>260662915.7224784</v>
+        <v>188787565951.3305</v>
       </c>
       <c r="E32" t="n">
-        <v>6072512.526771003</v>
+        <v>10977781767.50235</v>
       </c>
     </row>
     <row r="33">
@@ -993,16 +993,16 @@
         <v>44958</v>
       </c>
       <c r="B33" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C33" t="n">
-        <v>7.002427314665733</v>
+        <v>1586.539576583691</v>
       </c>
       <c r="D33" t="n">
-        <v>273619618.8753656</v>
+        <v>191042852121.4713</v>
       </c>
       <c r="E33" t="n">
-        <v>7488235.60185759</v>
+        <v>7544090211.946499</v>
       </c>
     </row>
     <row r="34">
@@ -1010,16 +1010,16 @@
         <v>44959</v>
       </c>
       <c r="B34" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C34" t="n">
-        <v>7.018549157088647</v>
+        <v>1642.857168158598</v>
       </c>
       <c r="D34" t="n">
-        <v>274861087.7252851</v>
+        <v>197724834027.5596</v>
       </c>
       <c r="E34" t="n">
-        <v>12033176.82081792</v>
+        <v>9295116915.9373</v>
       </c>
     </row>
     <row r="35">
@@ -1027,16 +1027,16 @@
         <v>44960</v>
       </c>
       <c r="B35" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C35" t="n">
-        <v>7.098171042474871</v>
+        <v>1648.679684076872</v>
       </c>
       <c r="D35" t="n">
-        <v>278165649.8527645</v>
+        <v>198613736403.1506</v>
       </c>
       <c r="E35" t="n">
-        <v>6560066.124715027</v>
+        <v>12542560274.34266</v>
       </c>
     </row>
     <row r="36">
@@ -1044,16 +1044,16 @@
         <v>44961</v>
       </c>
       <c r="B36" t="n">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C36" t="n">
-        <v>7.079972253476339</v>
+        <v>1665.427871223862</v>
       </c>
       <c r="D36" t="n">
-        <v>277678636.3971233</v>
+        <v>200784153460.4711</v>
       </c>
       <c r="E36" t="n">
-        <v>8381807.98982042</v>
+        <v>9528083087.520357</v>
       </c>
     </row>
     <row r="37">
@@ -1061,16 +1061,16 @@
         <v>44962</v>
       </c>
       <c r="B37" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C37" t="n">
-        <v>6.88157195542897</v>
+        <v>1667.271692563701</v>
       </c>
       <c r="D37" t="n">
-        <v>269689073.5506588</v>
+        <v>201099652782.7474</v>
       </c>
       <c r="E37" t="n">
-        <v>8553222.145380784</v>
+        <v>6766208820.07522</v>
       </c>
     </row>
     <row r="38">
@@ -1078,16 +1078,16 @@
         <v>44963</v>
       </c>
       <c r="B38" t="n">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C38" t="n">
-        <v>6.820536241110606</v>
+        <v>1631.372523363653</v>
       </c>
       <c r="D38" t="n">
-        <v>266335671.4993968</v>
+        <v>196817854756.2207</v>
       </c>
       <c r="E38" t="n">
-        <v>5440908.465682427</v>
+        <v>8211226952.330717</v>
       </c>
     </row>
     <row r="39">
@@ -1095,16 +1095,16 @@
         <v>44964</v>
       </c>
       <c r="B39" t="n">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C39" t="n">
-        <v>7.175474079253869</v>
+        <v>1617.144163289206</v>
       </c>
       <c r="D39" t="n">
-        <v>281580389.8524253</v>
+        <v>194725338782.4147</v>
       </c>
       <c r="E39" t="n">
-        <v>8854107.325984646</v>
+        <v>7825100535.008893</v>
       </c>
     </row>
     <row r="40">
@@ -1112,16 +1112,16 @@
         <v>44965</v>
       </c>
       <c r="B40" t="n">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C40" t="n">
-        <v>6.972659507662349</v>
+        <v>1672.822677775814</v>
       </c>
       <c r="D40" t="n">
-        <v>272908712.7487904</v>
+        <v>201779050385.8602</v>
       </c>
       <c r="E40" t="n">
-        <v>9144404.668373561</v>
+        <v>9180247305.88792</v>
       </c>
     </row>
     <row r="41">
@@ -1129,16 +1129,16 @@
         <v>44966</v>
       </c>
       <c r="B41" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C41" t="n">
-        <v>6.394938625027862</v>
+        <v>1651.40837860238</v>
       </c>
       <c r="D41" t="n">
-        <v>250417416.7727184</v>
+        <v>199107556553.1594</v>
       </c>
       <c r="E41" t="n">
-        <v>13626072.05101745</v>
+        <v>8766845417.320044</v>
       </c>
     </row>
     <row r="42">
@@ -1146,16 +1146,16 @@
         <v>44967</v>
       </c>
       <c r="B42" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C42" t="n">
-        <v>6.347036675904046</v>
+        <v>1546.383768658398</v>
       </c>
       <c r="D42" t="n">
-        <v>249365397.223714</v>
+        <v>186306817307.0956</v>
       </c>
       <c r="E42" t="n">
-        <v>5942335.009582</v>
+        <v>12447757846.41687</v>
       </c>
     </row>
     <row r="43">
@@ -1163,16 +1163,16 @@
         <v>44968</v>
       </c>
       <c r="B43" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C43" t="n">
-        <v>6.42516465672647</v>
+        <v>1515.534026861553</v>
       </c>
       <c r="D43" t="n">
-        <v>252526947.5332235</v>
+        <v>182839491763.3784</v>
       </c>
       <c r="E43" t="n">
-        <v>3541462.853798772</v>
+        <v>9882779899.96751</v>
       </c>
     </row>
     <row r="44">
@@ -1180,16 +1180,16 @@
         <v>44969</v>
       </c>
       <c r="B44" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C44" t="n">
-        <v>6.26760187037317</v>
+        <v>1541.968876941271</v>
       </c>
       <c r="D44" t="n">
-        <v>246731228.1337855</v>
+        <v>185826666441.3843</v>
       </c>
       <c r="E44" t="n">
-        <v>4779601.276076086</v>
+        <v>6070233325.97355</v>
       </c>
     </row>
     <row r="45">
@@ -1197,16 +1197,16 @@
         <v>44970</v>
       </c>
       <c r="B45" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C45" t="n">
-        <v>6.279481357912418</v>
+        <v>1515.33463118064</v>
       </c>
       <c r="D45" t="n">
-        <v>246522098.0506542</v>
+        <v>182722050130.9965</v>
       </c>
       <c r="E45" t="n">
-        <v>5732253.057591608</v>
+        <v>6128794710.192691</v>
       </c>
     </row>
     <row r="46">
@@ -1214,16 +1214,16 @@
         <v>44971</v>
       </c>
       <c r="B46" t="n">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C46" t="n">
-        <v>6.428742119553954</v>
+        <v>1506.916201013505</v>
       </c>
       <c r="D46" t="n">
-        <v>253458044.1931038</v>
+        <v>181589830341.348</v>
       </c>
       <c r="E46" t="n">
-        <v>6807600.004492456</v>
+        <v>11573812955.97068</v>
       </c>
     </row>
     <row r="47">
@@ -1231,16 +1231,16 @@
         <v>44972</v>
       </c>
       <c r="B47" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C47" t="n">
-        <v>7.281311736276288</v>
+        <v>1556.963484345393</v>
       </c>
       <c r="D47" t="n">
-        <v>286288484.4557377</v>
+        <v>187619568130.7347</v>
       </c>
       <c r="E47" t="n">
-        <v>104414041.2574906</v>
+        <v>11723184974.30426</v>
       </c>
     </row>
     <row r="48">
@@ -1248,16 +1248,16 @@
         <v>44973</v>
       </c>
       <c r="B48" t="n">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C48" t="n">
-        <v>7.067800441371491</v>
+        <v>1674.858207473528</v>
       </c>
       <c r="D48" t="n">
-        <v>277715146.953072</v>
+        <v>201595282287.4858</v>
       </c>
       <c r="E48" t="n">
-        <v>15999561.77945547</v>
+        <v>11079231384.24542</v>
       </c>
     </row>
     <row r="49">
@@ -1265,16 +1265,16 @@
         <v>44974</v>
       </c>
       <c r="B49" t="n">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C49" t="n">
-        <v>7.250157206601992</v>
+        <v>1646.143501886728</v>
       </c>
       <c r="D49" t="n">
-        <v>285781454.4514518</v>
+        <v>198370400841.4434</v>
       </c>
       <c r="E49" t="n">
-        <v>7934607.39920047</v>
+        <v>13388835215.08776</v>
       </c>
     </row>
     <row r="50">
@@ -1282,16 +1282,16 @@
         <v>44975</v>
       </c>
       <c r="B50" t="n">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C50" t="n">
-        <v>7.37323192006369</v>
+        <v>1697.084866573789</v>
       </c>
       <c r="D50" t="n">
-        <v>290555512.9097016</v>
+        <v>204534589183.7981</v>
       </c>
       <c r="E50" t="n">
-        <v>4929315.836011931</v>
+        <v>10807323083.84196</v>
       </c>
     </row>
     <row r="51">
@@ -1299,16 +1299,16 @@
         <v>44976</v>
       </c>
       <c r="B51" t="n">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C51" t="n">
-        <v>7.265436849670981</v>
+        <v>1692.518962831222</v>
       </c>
       <c r="D51" t="n">
-        <v>287911351.1913528</v>
+        <v>203613145994.3606</v>
       </c>
       <c r="E51" t="n">
-        <v>10738820.44113997</v>
+        <v>5863446679.020431</v>
       </c>
     </row>
     <row r="52">
@@ -1316,16 +1316,16 @@
         <v>44977</v>
       </c>
       <c r="B52" t="n">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C52" t="n">
-        <v>7.52664549860785</v>
+        <v>1680.378685700073</v>
       </c>
       <c r="D52" t="n">
-        <v>297236320.6097583</v>
+        <v>202999098993.9826</v>
       </c>
       <c r="E52" t="n">
-        <v>12993337.24206771</v>
+        <v>7499517187.119554</v>
       </c>
     </row>
     <row r="53">
@@ -1333,16 +1333,16 @@
         <v>44978</v>
       </c>
       <c r="B53" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C53" t="n">
-        <v>7.2298789796956</v>
+        <v>1700.198681499266</v>
       </c>
       <c r="D53" t="n">
-        <v>285083713.0470961</v>
+        <v>204900256888.8414</v>
       </c>
       <c r="E53" t="n">
-        <v>9228477.66099239</v>
+        <v>8435810846.264387</v>
       </c>
     </row>
     <row r="54">
@@ -1350,16 +1350,16 @@
         <v>44979</v>
       </c>
       <c r="B54" t="n">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C54" t="n">
-        <v>7.12944129367671</v>
+        <v>1656.582369571119</v>
       </c>
       <c r="D54" t="n">
-        <v>282411838.7439171</v>
+        <v>199387951962.0551</v>
       </c>
       <c r="E54" t="n">
-        <v>8574018.866483158</v>
+        <v>9728814194.484383</v>
       </c>
     </row>
     <row r="55">
@@ -1367,16 +1367,16 @@
         <v>44980</v>
       </c>
       <c r="B55" t="n">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C55" t="n">
-        <v>7.274067547121122</v>
+        <v>1643.173393745349</v>
       </c>
       <c r="D55" t="n">
-        <v>287334779.7908815</v>
+        <v>198153971276.3559</v>
       </c>
       <c r="E55" t="n">
-        <v>11069922.27378555</v>
+        <v>9836391621.850903</v>
       </c>
     </row>
     <row r="56">
@@ -1384,16 +1384,16 @@
         <v>44981</v>
       </c>
       <c r="B56" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C56" t="n">
-        <v>7.032901261250053</v>
+        <v>1651.850006691427</v>
       </c>
       <c r="D56" t="n">
-        <v>278441316.4545644</v>
+        <v>198619189860.0559</v>
       </c>
       <c r="E56" t="n">
-        <v>9715397.264744021</v>
+        <v>9698749201.902168</v>
       </c>
     </row>
     <row r="57">
@@ -1401,16 +1401,16 @@
         <v>44982</v>
       </c>
       <c r="B57" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C57" t="n">
-        <v>6.977650889701508</v>
+        <v>1608.103493653836</v>
       </c>
       <c r="D57" t="n">
-        <v>276204692.1973316</v>
+        <v>193773223390.3348</v>
       </c>
       <c r="E57" t="n">
-        <v>4796026.159308838</v>
+        <v>9609840835.076471</v>
       </c>
     </row>
     <row r="58">
@@ -1418,16 +1418,16 @@
         <v>44983</v>
       </c>
       <c r="B58" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C58" t="n">
-        <v>7.095025140359082</v>
+        <v>1593.951973790846</v>
       </c>
       <c r="D58" t="n">
-        <v>281058362.6289822</v>
+        <v>192056375721.2107</v>
       </c>
       <c r="E58" t="n">
-        <v>3659384.655612133</v>
+        <v>6117521125.045025</v>
       </c>
     </row>
     <row r="59">
@@ -1435,16 +1435,16 @@
         <v>44984</v>
       </c>
       <c r="B59" t="n">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C59" t="n">
-        <v>7.039595614360527</v>
+        <v>1640.582710194306</v>
       </c>
       <c r="D59" t="n">
-        <v>278758184.0558037</v>
+        <v>197696596339.3676</v>
       </c>
       <c r="E59" t="n">
-        <v>5759337.00826832</v>
+        <v>6357994998.206232</v>
       </c>
     </row>
     <row r="60">
@@ -1452,16 +1452,16 @@
         <v>44985</v>
       </c>
       <c r="B60" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C60" t="n">
-        <v>7.065107037991336</v>
+        <v>1633.976628983382</v>
       </c>
       <c r="D60" t="n">
-        <v>280203647.2631443</v>
+        <v>197018105507.0607</v>
       </c>
       <c r="E60" t="n">
-        <v>13441868.82985036</v>
+        <v>7916573299.24559</v>
       </c>
     </row>
     <row r="61">
@@ -1469,16 +1469,16 @@
         <v>44986</v>
       </c>
       <c r="B61" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C61" t="n">
-        <v>7.213782471287141</v>
+        <v>1606.632639454843</v>
       </c>
       <c r="D61" t="n">
-        <v>285957389.3009415</v>
+        <v>193276888983.6779</v>
       </c>
       <c r="E61" t="n">
-        <v>58955994.36646608</v>
+        <v>6883711561.9226</v>
       </c>
     </row>
     <row r="62">
@@ -1486,16 +1486,16 @@
         <v>44987</v>
       </c>
       <c r="B62" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C62" t="n">
-        <v>6.965686899137807</v>
+        <v>1663.925777294461</v>
       </c>
       <c r="D62" t="n">
-        <v>276630053.7287742</v>
+        <v>200476156508.3419</v>
       </c>
       <c r="E62" t="n">
-        <v>9487528.555922346</v>
+        <v>8672222866.055677</v>
       </c>
     </row>
     <row r="63">
@@ -1503,16 +1503,16 @@
         <v>44988</v>
       </c>
       <c r="B63" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C63" t="n">
-        <v>6.503757052710228</v>
+        <v>1647.664666907772</v>
       </c>
       <c r="D63" t="n">
-        <v>258263438.7044892</v>
+        <v>198520753673.5454</v>
       </c>
       <c r="E63" t="n">
-        <v>10582892.39124615</v>
+        <v>7930395056.206914</v>
       </c>
     </row>
     <row r="64">
@@ -1520,16 +1520,16 @@
         <v>44989</v>
       </c>
       <c r="B64" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C64" t="n">
-        <v>6.383642131572313</v>
+        <v>1570.668210599776</v>
       </c>
       <c r="D64" t="n">
-        <v>253823751.059809</v>
+        <v>189178795460.2609</v>
       </c>
       <c r="E64" t="n">
-        <v>7847700.82781959</v>
+        <v>11179316252.20772</v>
       </c>
     </row>
     <row r="65">
@@ -1537,16 +1537,16 @@
         <v>44990</v>
       </c>
       <c r="B65" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C65" t="n">
-        <v>6.347408512367774</v>
+        <v>1568.495601056219</v>
       </c>
       <c r="D65" t="n">
-        <v>252137587.0770049</v>
+        <v>189002414068.6852</v>
       </c>
       <c r="E65" t="n">
-        <v>6894889.830517531</v>
+        <v>4800994312.370927</v>
       </c>
     </row>
     <row r="66">
@@ -1554,16 +1554,16 @@
         <v>44991</v>
       </c>
       <c r="B66" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C66" t="n">
-        <v>6.400741640122369</v>
+        <v>1563.22566200563</v>
       </c>
       <c r="D66" t="n">
-        <v>254705209.4660594</v>
+        <v>188337456156.2138</v>
       </c>
       <c r="E66" t="n">
-        <v>6412358.666467028</v>
+        <v>62172854406.22754</v>
       </c>
     </row>
     <row r="67">
@@ -1571,16 +1571,16 @@
         <v>44992</v>
       </c>
       <c r="B67" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C67" t="n">
-        <v>6.322668910767872</v>
+        <v>1567.350146525219</v>
       </c>
       <c r="D67" t="n">
-        <v>251301182.145392</v>
+        <v>188803304807.8448</v>
       </c>
       <c r="E67" t="n">
-        <v>5125733.271645633</v>
+        <v>6627693313.532333</v>
       </c>
     </row>
     <row r="68">
@@ -1588,16 +1588,16 @@
         <v>44993</v>
       </c>
       <c r="B68" t="n">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C68" t="n">
-        <v>6.1673061324981</v>
+        <v>1563.813182247501</v>
       </c>
       <c r="D68" t="n">
-        <v>245594642.1610681</v>
+        <v>187945419858.8607</v>
       </c>
       <c r="E68" t="n">
-        <v>10637637.35398656</v>
+        <v>8523808476.527845</v>
       </c>
     </row>
     <row r="69">
@@ -1605,16 +1605,16 @@
         <v>44994</v>
       </c>
       <c r="B69" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C69" t="n">
-        <v>5.725591326175225</v>
+        <v>1535.26025209711</v>
       </c>
       <c r="D69" t="n">
-        <v>227893120.3706616</v>
+        <v>185138878803.2572</v>
       </c>
       <c r="E69" t="n">
-        <v>5182454.603044959</v>
+        <v>11881879818.72524</v>
       </c>
     </row>
     <row r="70">
@@ -1622,16 +1622,16 @@
         <v>44995</v>
       </c>
       <c r="B70" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C70" t="n">
-        <v>5.659354027016782</v>
+        <v>1440.167661880184</v>
       </c>
       <c r="D70" t="n">
-        <v>225665255.1189694</v>
+        <v>173232609854.2885</v>
       </c>
       <c r="E70" t="n">
-        <v>6235027.138800535</v>
+        <v>10861201441.13542</v>
       </c>
     </row>
     <row r="71">
@@ -1639,16 +1639,16 @@
         <v>44996</v>
       </c>
       <c r="B71" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C71" t="n">
-        <v>5.774292256932373</v>
+        <v>1429.603169104185</v>
       </c>
       <c r="D71" t="n">
-        <v>229841016.3580246</v>
+        <v>172474466355.7147</v>
       </c>
       <c r="E71" t="n">
-        <v>7115882.974864691</v>
+        <v>14696381616.84098</v>
       </c>
     </row>
     <row r="72">
@@ -1656,16 +1656,16 @@
         <v>44997</v>
       </c>
       <c r="B72" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C72" t="n">
-        <v>6.396515744030597</v>
+        <v>1474.40324440156</v>
       </c>
       <c r="D72" t="n">
-        <v>254755940.8469577</v>
+        <v>176915178456.4187</v>
       </c>
       <c r="E72" t="n">
-        <v>10346019.6152311</v>
+        <v>18345198261.39598</v>
       </c>
     </row>
     <row r="73">
@@ -1673,16 +1673,16 @@
         <v>44998</v>
       </c>
       <c r="B73" t="n">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C73" t="n">
-        <v>6.583666777626488</v>
+        <v>1588.196802053047</v>
       </c>
       <c r="D73" t="n">
-        <v>263296047.5062894</v>
+        <v>190440681263.2129</v>
       </c>
       <c r="E73" t="n">
-        <v>7931297.143035312</v>
+        <v>13967891188.5</v>
       </c>
     </row>
     <row r="74">
@@ -1690,16 +1690,16 @@
         <v>44999</v>
       </c>
       <c r="B74" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C74" t="n">
-        <v>6.759034779430099</v>
+        <v>1678.915634393308</v>
       </c>
       <c r="D74" t="n">
-        <v>269935566.8572126</v>
+        <v>202294154847.0903</v>
       </c>
       <c r="E74" t="n">
-        <v>11018024.62436139</v>
+        <v>65211714924.50838</v>
       </c>
     </row>
     <row r="75">
@@ -1707,16 +1707,16 @@
         <v>45000</v>
       </c>
       <c r="B75" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C75" t="n">
-        <v>6.320257542079611</v>
+        <v>1708.300897366666</v>
       </c>
       <c r="D75" t="n">
-        <v>252542646.526623</v>
+        <v>205738833552.6543</v>
       </c>
       <c r="E75" t="n">
-        <v>9701019.657138605</v>
+        <v>19833762797.58361</v>
       </c>
     </row>
     <row r="76">
@@ -1724,16 +1724,16 @@
         <v>45001</v>
       </c>
       <c r="B76" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C76" t="n">
-        <v>6.384446716150901</v>
+        <v>1658.070108566312</v>
       </c>
       <c r="D76" t="n">
-        <v>255788614.0444269</v>
+        <v>199607487558.3324</v>
       </c>
       <c r="E76" t="n">
-        <v>5108528.436649034</v>
+        <v>17257648020.36215</v>
       </c>
     </row>
     <row r="77">
@@ -1741,16 +1741,16 @@
         <v>45002</v>
       </c>
       <c r="B77" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C77" t="n">
-        <v>6.777406805762209</v>
+        <v>1679.79247620809</v>
       </c>
       <c r="D77" t="n">
-        <v>270759812.6424067</v>
+        <v>202411234958.1569</v>
       </c>
       <c r="E77" t="n">
-        <v>5145022.98068116</v>
+        <v>30201930394.76128</v>
       </c>
     </row>
     <row r="78">
@@ -1758,16 +1758,16 @@
         <v>45003</v>
       </c>
       <c r="B78" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C78" t="n">
-        <v>6.736087637489586</v>
+        <v>1793.298801734233</v>
       </c>
       <c r="D78" t="n">
-        <v>269851956.9045601</v>
+        <v>215660560704.7752</v>
       </c>
       <c r="E78" t="n">
-        <v>9541109.045494255</v>
+        <v>14459727611.04181</v>
       </c>
     </row>
     <row r="79">
@@ -1775,16 +1775,16 @@
         <v>45004</v>
       </c>
       <c r="B79" t="n">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C79" t="n">
-        <v>6.780797076440868</v>
+        <v>1769.425326912385</v>
       </c>
       <c r="D79" t="n">
-        <v>272723016.0051329</v>
+        <v>213123927233.328</v>
       </c>
       <c r="E79" t="n">
-        <v>7701317.072631557</v>
+        <v>11976182095.29605</v>
       </c>
     </row>
     <row r="80">
@@ -1792,16 +1792,16 @@
         <v>45005</v>
       </c>
       <c r="B80" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C80" t="n">
-        <v>6.558197385470811</v>
+        <v>1801.367419011459</v>
       </c>
       <c r="D80" t="n">
-        <v>262557923.718209</v>
+        <v>217844457987.9951</v>
       </c>
       <c r="E80" t="n">
-        <v>4383554.365777608</v>
+        <v>10745813975.10349</v>
       </c>
     </row>
     <row r="81">
@@ -1809,16 +1809,16 @@
         <v>45006</v>
       </c>
       <c r="B81" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C81" t="n">
-        <v>6.782283528550663</v>
+        <v>1744.441459960018</v>
       </c>
       <c r="D81" t="n">
-        <v>271685118.9734492</v>
+        <v>209763828559.9232</v>
       </c>
       <c r="E81" t="n">
-        <v>5517861.413514332</v>
+        <v>12973595973.35999</v>
       </c>
     </row>
     <row r="82">
@@ -1826,16 +1826,16 @@
         <v>45007</v>
       </c>
       <c r="B82" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C82" t="n">
-        <v>6.594043047672288</v>
+        <v>1811.411243668274</v>
       </c>
       <c r="D82" t="n">
-        <v>264256631.4187802</v>
+        <v>218008486913.6836</v>
       </c>
       <c r="E82" t="n">
-        <v>4005944.354583108</v>
+        <v>10831022955.19994</v>
       </c>
     </row>
     <row r="83">
@@ -1843,16 +1843,16 @@
         <v>45008</v>
       </c>
       <c r="B83" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C83" t="n">
-        <v>7.084532777561027</v>
+        <v>1747.640028114114</v>
       </c>
       <c r="D83" t="n">
-        <v>284404298.6401306</v>
+        <v>210285658211.0843</v>
       </c>
       <c r="E83" t="n">
-        <v>10084604.56075571</v>
+        <v>13820716099.50186</v>
       </c>
     </row>
     <row r="84">
@@ -1860,16 +1860,16 @@
         <v>45009</v>
       </c>
       <c r="B84" t="n">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C84" t="n">
-        <v>6.551036831375837</v>
+        <v>1824.956657894933</v>
       </c>
       <c r="D84" t="n">
-        <v>264581457.6714334</v>
+        <v>219518418514.1925</v>
       </c>
       <c r="E84" t="n">
-        <v>6526037.209866154</v>
+        <v>10980967034.93774</v>
       </c>
     </row>
     <row r="85">
@@ -1877,16 +1877,16 @@
         <v>45010</v>
       </c>
       <c r="B85" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C85" t="n">
-        <v>6.717545205123711</v>
+        <v>1751.219407826173</v>
       </c>
       <c r="D85" t="n">
-        <v>269396040.1644043</v>
+        <v>212072713258.261</v>
       </c>
       <c r="E85" t="n">
-        <v>6514341.651255416</v>
+        <v>11601017881.78658</v>
       </c>
     </row>
     <row r="86">
@@ -1894,16 +1894,16 @@
         <v>45011</v>
       </c>
       <c r="B86" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C86" t="n">
-        <v>6.813133557321466</v>
+        <v>1753.982636507409</v>
       </c>
       <c r="D86" t="n">
-        <v>274340082.6564069</v>
+        <v>211355889911.3326</v>
       </c>
       <c r="E86" t="n">
-        <v>3215998.143334421</v>
+        <v>8023849174.389528</v>
       </c>
     </row>
     <row r="87">
@@ -1911,16 +1911,16 @@
         <v>45012</v>
       </c>
       <c r="B87" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C87" t="n">
-        <v>6.482214424094255</v>
+        <v>1776.867690456723</v>
       </c>
       <c r="D87" t="n">
-        <v>260240672.2274781</v>
+        <v>214528709136.8291</v>
       </c>
       <c r="E87" t="n">
-        <v>7038859.817899136</v>
+        <v>8417258785.455161</v>
       </c>
     </row>
     <row r="88">
@@ -1928,16 +1928,16 @@
         <v>45013</v>
       </c>
       <c r="B88" t="n">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C88" t="n">
-        <v>6.911380143612694</v>
+        <v>1719.170972674861</v>
       </c>
       <c r="D88" t="n">
-        <v>277653963.1553106</v>
+        <v>206685090340.5369</v>
       </c>
       <c r="E88" t="n">
-        <v>11964059.7071323</v>
+        <v>9757415238.165146</v>
       </c>
     </row>
     <row r="89">
@@ -1945,16 +1945,16 @@
         <v>45014</v>
       </c>
       <c r="B89" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C89" t="n">
-        <v>6.914038839058302</v>
+        <v>1776.043639329832</v>
       </c>
       <c r="D89" t="n">
-        <v>278273496.1270115</v>
+        <v>213909228254.6471</v>
       </c>
       <c r="E89" t="n">
-        <v>11807195.84690091</v>
+        <v>9548011563.716631</v>
       </c>
     </row>
     <row r="90">
@@ -1962,16 +1962,16 @@
         <v>45015</v>
       </c>
       <c r="B90" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C90" t="n">
-        <v>6.827821458747403</v>
+        <v>1795.536947827324</v>
       </c>
       <c r="D90" t="n">
-        <v>274946683.6055182</v>
+        <v>216268184816.8208</v>
       </c>
       <c r="E90" t="n">
-        <v>6413987.542611027</v>
+        <v>10395388838.76884</v>
       </c>
     </row>
     <row r="91">
@@ -1979,16 +1979,16 @@
         <v>45016</v>
       </c>
       <c r="B91" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C91" t="n">
-        <v>6.970098508360446</v>
+        <v>1792.908578308043</v>
       </c>
       <c r="D91" t="n">
-        <v>281496968.8817041</v>
+        <v>216024475834.1531</v>
       </c>
       <c r="E91" t="n">
-        <v>20390540.86081478</v>
+        <v>10958214915.4279</v>
       </c>
     </row>
     <row r="92">
@@ -1996,16 +1996,16 @@
         <v>45017</v>
       </c>
       <c r="B92" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C92" t="n">
-        <v>6.98492289380657</v>
+        <v>1824.020005552818</v>
       </c>
       <c r="D92" t="n">
-        <v>281701212.4118622</v>
+        <v>219903281108.4414</v>
       </c>
       <c r="E92" t="n">
-        <v>5514271.332036392</v>
+        <v>10329452626.6318</v>
       </c>
     </row>
     <row r="93">
@@ -2013,16 +2013,16 @@
         <v>45018</v>
       </c>
       <c r="B93" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C93" t="n">
-        <v>6.822725481152257</v>
+        <v>1823.000379825308</v>
       </c>
       <c r="D93" t="n">
-        <v>274831850.4905782</v>
+        <v>219561711559.01</v>
       </c>
       <c r="E93" t="n">
-        <v>5162070.312530654</v>
+        <v>6199278060.289369</v>
       </c>
     </row>
     <row r="94">
@@ -2030,16 +2030,16 @@
         <v>45019</v>
       </c>
       <c r="B94" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C94" t="n">
-        <v>6.771301310706908</v>
+        <v>1797.736988393855</v>
       </c>
       <c r="D94" t="n">
-        <v>273604632.1857387</v>
+        <v>216494189054.4792</v>
       </c>
       <c r="E94" t="n">
-        <v>7796620.322914717</v>
+        <v>6679784659.59878</v>
       </c>
     </row>
     <row r="95">
@@ -2047,16 +2047,16 @@
         <v>45020</v>
       </c>
       <c r="B95" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C95" t="n">
-        <v>6.990790024040606</v>
+        <v>1810.466255484756</v>
       </c>
       <c r="D95" t="n">
-        <v>281982939.9619054</v>
+        <v>218499091537.9477</v>
       </c>
       <c r="E95" t="n">
-        <v>4868362.181193078</v>
+        <v>11141583996.17221</v>
       </c>
     </row>
     <row r="96">
@@ -2064,16 +2064,16 @@
         <v>45021</v>
       </c>
       <c r="B96" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C96" t="n">
-        <v>7.287893360803872</v>
+        <v>1871.333525898643</v>
       </c>
       <c r="D96" t="n">
-        <v>294291487.377271</v>
+        <v>225257854355.9486</v>
       </c>
       <c r="E96" t="n">
-        <v>5412847.594434462</v>
+        <v>11580514457.96186</v>
       </c>
     </row>
     <row r="97">
@@ -2081,16 +2081,16 @@
         <v>45022</v>
       </c>
       <c r="B97" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C97" t="n">
-        <v>7.103216301183756</v>
+        <v>1911.338689951751</v>
       </c>
       <c r="D97" t="n">
-        <v>286642143.257203</v>
+        <v>230370056366.2714</v>
       </c>
       <c r="E97" t="n">
-        <v>4219156.47286575</v>
+        <v>11586484696.70598</v>
       </c>
     </row>
     <row r="98">
@@ -2098,16 +2098,16 @@
         <v>45023</v>
       </c>
       <c r="B98" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C98" t="n">
-        <v>7.074743252141506</v>
+        <v>1872.246682367909</v>
       </c>
       <c r="D98" t="n">
-        <v>286157404.6018183</v>
+        <v>225549620778.9139</v>
       </c>
       <c r="E98" t="n">
-        <v>3897535.247567709</v>
+        <v>9208408844.045069</v>
       </c>
     </row>
     <row r="99">
@@ -2115,16 +2115,16 @@
         <v>45024</v>
       </c>
       <c r="B99" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C99" t="n">
-        <v>6.903033746329151</v>
+        <v>1866.657544787415</v>
       </c>
       <c r="D99" t="n">
-        <v>279180552.786694</v>
+        <v>224884695655.0538</v>
       </c>
       <c r="E99" t="n">
-        <v>3869494.782953831</v>
+        <v>9298216041.371656</v>
       </c>
     </row>
     <row r="100">
@@ -2132,16 +2132,16 @@
         <v>45025</v>
       </c>
       <c r="B100" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C100" t="n">
-        <v>6.969054218758775</v>
+        <v>1851.050671070621</v>
       </c>
       <c r="D100" t="n">
-        <v>281896593.4944839</v>
+        <v>223169245107.383</v>
       </c>
       <c r="E100" t="n">
-        <v>3573390.790596966</v>
+        <v>5970294474.952573</v>
       </c>
     </row>
     <row r="101">
@@ -2149,16 +2149,16 @@
         <v>45026</v>
       </c>
       <c r="B101" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C101" t="n">
-        <v>7.296754594254579</v>
+        <v>1859.940387287814</v>
       </c>
       <c r="D101" t="n">
-        <v>295709724.5183633</v>
+        <v>224219517643.8137</v>
       </c>
       <c r="E101" t="n">
-        <v>7323346.859704349</v>
+        <v>7405572878.99046</v>
       </c>
     </row>
     <row r="102">
@@ -2166,16 +2166,16 @@
         <v>45027</v>
       </c>
       <c r="B102" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C102" t="n">
-        <v>7.016962512090705</v>
+        <v>1909.882060941591</v>
       </c>
       <c r="D102" t="n">
-        <v>284108703.636039</v>
+        <v>230201702660.8635</v>
       </c>
       <c r="E102" t="n">
-        <v>5875974.495135708</v>
+        <v>9639736045.970774</v>
       </c>
     </row>
     <row r="103">
@@ -2183,16 +2183,16 @@
         <v>45028</v>
       </c>
       <c r="B103" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C103" t="n">
-        <v>6.947780185536482</v>
+        <v>1892.938911069582</v>
       </c>
       <c r="D103" t="n">
-        <v>281789894.7803555</v>
+        <v>227988460702.9362</v>
       </c>
       <c r="E103" t="n">
-        <v>7130037.41054859</v>
+        <v>10245367683.71216</v>
       </c>
     </row>
     <row r="104">
@@ -2200,16 +2200,16 @@
         <v>45029</v>
       </c>
       <c r="B104" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C104" t="n">
-        <v>7.229104517389263</v>
+        <v>1920.223031193122</v>
       </c>
       <c r="D104" t="n">
-        <v>293316971.8043993</v>
+        <v>231476399968.9067</v>
       </c>
       <c r="E104" t="n">
-        <v>6479819.960938787</v>
+        <v>13152150835.22722</v>
       </c>
     </row>
     <row r="105">
@@ -2217,16 +2217,16 @@
         <v>45030</v>
       </c>
       <c r="B105" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C105" t="n">
-        <v>7.200469300608165</v>
+        <v>2012.785415162006</v>
       </c>
       <c r="D105" t="n">
-        <v>291975176.0106083</v>
+        <v>242284529486.3431</v>
       </c>
       <c r="E105" t="n">
-        <v>14987117.40090008</v>
+        <v>13956404022.5792</v>
       </c>
     </row>
     <row r="106">
@@ -2234,16 +2234,16 @@
         <v>45031</v>
       </c>
       <c r="B106" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C106" t="n">
-        <v>7.22998525572962</v>
+        <v>2102.946188294908</v>
       </c>
       <c r="D106" t="n">
-        <v>293813284.8334792</v>
+        <v>252719453976.0147</v>
       </c>
       <c r="E106" t="n">
-        <v>6002143.582139045</v>
+        <v>17899705467.09288</v>
       </c>
     </row>
     <row r="107">
@@ -2251,16 +2251,16 @@
         <v>45032</v>
       </c>
       <c r="B107" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C107" t="n">
-        <v>7.215731160934795</v>
+        <v>2093.166331331955</v>
       </c>
       <c r="D107" t="n">
-        <v>292689999.8747999</v>
+        <v>251586840869.9989</v>
       </c>
       <c r="E107" t="n">
-        <v>4710716.750620043</v>
+        <v>9272832786.084044</v>
       </c>
     </row>
     <row r="108">
@@ -2268,16 +2268,16 @@
         <v>45033</v>
       </c>
       <c r="B108" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C108" t="n">
-        <v>7.128154727940786</v>
+        <v>2118.598789153885</v>
       </c>
       <c r="D108" t="n">
-        <v>289545096.1282432</v>
+        <v>253507799906.4971</v>
       </c>
       <c r="E108" t="n">
-        <v>5514048.831594138</v>
+        <v>8879608633.84169</v>
       </c>
     </row>
     <row r="109">
@@ -2285,16 +2285,16 @@
         <v>45034</v>
       </c>
       <c r="B109" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C109" t="n">
-        <v>7.124470430161402</v>
+        <v>2077.535664637183</v>
       </c>
       <c r="D109" t="n">
-        <v>289297335.6509632</v>
+        <v>247900016291.376</v>
       </c>
       <c r="E109" t="n">
-        <v>5843715.832981437</v>
+        <v>10818847581.54074</v>
       </c>
     </row>
     <row r="110">
@@ -2302,16 +2302,16 @@
         <v>45035</v>
       </c>
       <c r="B110" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C110" t="n">
-        <v>6.490844610813437</v>
+        <v>2103.278813592151</v>
       </c>
       <c r="D110" t="n">
-        <v>263823754.9868762</v>
+        <v>251100187595.887</v>
       </c>
       <c r="E110" t="n">
-        <v>9274597.206955822</v>
+        <v>10121134598.14348</v>
       </c>
     </row>
     <row r="111">
@@ -2319,16 +2319,16 @@
         <v>45036</v>
       </c>
       <c r="B111" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C111" t="n">
-        <v>6.468927540903823</v>
+        <v>1936.425920798363</v>
       </c>
       <c r="D111" t="n">
-        <v>262844712.999613</v>
+        <v>231458322403.7939</v>
       </c>
       <c r="E111" t="n">
-        <v>10325552.09616121</v>
+        <v>15695628542.02445</v>
       </c>
     </row>
     <row r="112">
@@ -2336,16 +2336,16 @@
         <v>45037</v>
       </c>
       <c r="B112" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C112" t="n">
-        <v>6.06627967247289</v>
+        <v>1943.435598192578</v>
       </c>
       <c r="D112" t="n">
-        <v>246706771.6834139</v>
+        <v>233965107542.7419</v>
       </c>
       <c r="E112" t="n">
-        <v>6887871.115547808</v>
+        <v>12422352272.16522</v>
       </c>
     </row>
     <row r="113">
@@ -2353,16 +2353,16 @@
         <v>45038</v>
       </c>
       <c r="B113" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C113" t="n">
-        <v>6.180741213473991</v>
+        <v>1850.149738424215</v>
       </c>
       <c r="D113" t="n">
-        <v>251246401.9782337</v>
+        <v>222536195564.3714</v>
       </c>
       <c r="E113" t="n">
-        <v>5905866.284953683</v>
+        <v>13427480065.76744</v>
       </c>
     </row>
     <row r="114">
@@ -2370,16 +2370,16 @@
         <v>45039</v>
       </c>
       <c r="B114" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C114" t="n">
-        <v>6.150664560698109</v>
+        <v>1877.541328061146</v>
       </c>
       <c r="D114" t="n">
-        <v>249519573.6978379</v>
+        <v>226130094815.9329</v>
       </c>
       <c r="E114" t="n">
-        <v>5183926.668659622</v>
+        <v>7809497062.825459</v>
       </c>
     </row>
     <row r="115">
@@ -2387,16 +2387,16 @@
         <v>45040</v>
       </c>
       <c r="B115" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C115" t="n">
-        <v>5.977917364849882</v>
+        <v>1863.639142214224</v>
       </c>
       <c r="D115" t="n">
-        <v>243476740.3162035</v>
+        <v>224130103074.6425</v>
       </c>
       <c r="E115" t="n">
-        <v>6543684.898603891</v>
+        <v>7375382210.29527</v>
       </c>
     </row>
     <row r="116">
@@ -2404,16 +2404,16 @@
         <v>45041</v>
       </c>
       <c r="B116" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C116" t="n">
-        <v>6.175254762250034</v>
+        <v>1842.630792087157</v>
       </c>
       <c r="D116" t="n">
-        <v>250175000.3687885</v>
+        <v>221819334333.2904</v>
       </c>
       <c r="E116" t="n">
-        <v>5177848.286356026</v>
+        <v>9177916724.086399</v>
       </c>
     </row>
     <row r="117">
@@ -2421,16 +2421,16 @@
         <v>45042</v>
       </c>
       <c r="B117" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C117" t="n">
-        <v>6.080403232921645</v>
+        <v>1870.565223123027</v>
       </c>
       <c r="D117" t="n">
-        <v>248377978.29081</v>
+        <v>225096171581.735</v>
       </c>
       <c r="E117" t="n">
-        <v>8492196.379781134</v>
+        <v>9669740943.905441</v>
       </c>
     </row>
     <row r="118">
@@ -2438,16 +2438,16 @@
         <v>45043</v>
       </c>
       <c r="B118" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C118" t="n">
-        <v>6.21023758569446</v>
+        <v>1867.589325012487</v>
       </c>
       <c r="D118" t="n">
-        <v>252835551.3132612</v>
+        <v>224807445929.1713</v>
       </c>
       <c r="E118" t="n">
-        <v>5643410.549944057</v>
+        <v>16137081936.11856</v>
       </c>
     </row>
     <row r="119">
@@ -2455,16 +2455,16 @@
         <v>45044</v>
       </c>
       <c r="B119" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C119" t="n">
-        <v>6.072317677404537</v>
+        <v>1910.456779102895</v>
       </c>
       <c r="D119" t="n">
-        <v>247393706.8004263</v>
+        <v>229940294581.2185</v>
       </c>
       <c r="E119" t="n">
-        <v>5476130.176279615</v>
+        <v>17307261170.94721</v>
       </c>
     </row>
     <row r="120">
@@ -2472,16 +2472,16 @@
         <v>45045</v>
       </c>
       <c r="B120" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C120" t="n">
-        <v>6.12499323718404</v>
+        <v>1894.428083950107</v>
       </c>
       <c r="D120" t="n">
-        <v>250056045.0515924</v>
+        <v>228152292773.1309</v>
       </c>
       <c r="E120" t="n">
-        <v>3983287.358948038</v>
+        <v>8853391784.29081</v>
       </c>
     </row>
     <row r="121">
@@ -2489,16 +2489,16 @@
         <v>45046</v>
       </c>
       <c r="B121" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C121" t="n">
-        <v>6.026582537437334</v>
+        <v>1905.27385227321</v>
       </c>
       <c r="D121" t="n">
-        <v>247007262.8014638</v>
+        <v>229429843509.54</v>
       </c>
       <c r="E121" t="n">
-        <v>4909041.781279086</v>
+        <v>5262009753.405011</v>
       </c>
     </row>
     <row r="122">
@@ -2506,16 +2506,16 @@
         <v>45047</v>
       </c>
       <c r="B122" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C122" t="n">
-        <v>5.892534693629076</v>
+        <v>1885.391935336922</v>
       </c>
       <c r="D122" t="n">
-        <v>240219021.724574</v>
+        <v>227186562478.899</v>
       </c>
       <c r="E122" t="n">
-        <v>4794985.52370882</v>
+        <v>7328083478.977482</v>
       </c>
     </row>
     <row r="123">
@@ -2523,16 +2523,16 @@
         <v>45048</v>
       </c>
       <c r="B123" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C123" t="n">
-        <v>6.015680237139553</v>
+        <v>1832.725799406749</v>
       </c>
       <c r="D123" t="n">
-        <v>245284797.7535747</v>
+        <v>220608989107.972</v>
       </c>
       <c r="E123" t="n">
-        <v>4616285.604068668</v>
+        <v>9673378163.522745</v>
       </c>
     </row>
     <row r="124">
@@ -2540,16 +2540,16 @@
         <v>45049</v>
       </c>
       <c r="B124" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C124" t="n">
-        <v>6.12315112773214</v>
+        <v>1870.828572787594</v>
       </c>
       <c r="D124" t="n">
-        <v>250090773.7974523</v>
+        <v>225192198744.2643</v>
       </c>
       <c r="E124" t="n">
-        <v>4971163.2373866</v>
+        <v>8338110887.912115</v>
       </c>
     </row>
     <row r="125">
@@ -2557,16 +2557,16 @@
         <v>45050</v>
       </c>
       <c r="B125" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C125" t="n">
-        <v>6.058157809675603</v>
+        <v>1903.728210735278</v>
       </c>
       <c r="D125" t="n">
-        <v>247658592.252959</v>
+        <v>229058202737.1404</v>
       </c>
       <c r="E125" t="n">
-        <v>4684126.234649901</v>
+        <v>8855867548.894463</v>
       </c>
     </row>
     <row r="126">
@@ -2574,16 +2574,16 @@
         <v>45051</v>
       </c>
       <c r="B126" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C126" t="n">
-        <v>6.258602367236163</v>
+        <v>1877.401195052536</v>
       </c>
       <c r="D126" t="n">
-        <v>255240853.2789599</v>
+        <v>226033834100.1215</v>
       </c>
       <c r="E126" t="n">
-        <v>9293071.450204721</v>
+        <v>7156399180.62065</v>
       </c>
     </row>
     <row r="127">
@@ -2591,16 +2591,16 @@
         <v>45052</v>
       </c>
       <c r="B127" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C127" t="n">
-        <v>6.032274581407498</v>
+        <v>1993.612965747434</v>
       </c>
       <c r="D127" t="n">
-        <v>246993388.6294954</v>
+        <v>239911504424.294</v>
       </c>
       <c r="E127" t="n">
-        <v>9555785.234358383</v>
+        <v>10662067255.96863</v>
       </c>
     </row>
     <row r="128">
@@ -2608,16 +2608,16 @@
         <v>45053</v>
       </c>
       <c r="B128" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C128" t="n">
-        <v>6.018018176929921</v>
+        <v>1900.410599025731</v>
       </c>
       <c r="D128" t="n">
-        <v>245433719.8714863</v>
+        <v>228369002903.6794</v>
       </c>
       <c r="E128" t="n">
-        <v>8005885.308123725</v>
+        <v>11135926723.29712</v>
       </c>
     </row>
     <row r="129">
@@ -2625,16 +2625,16 @@
         <v>45054</v>
       </c>
       <c r="B129" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C129" t="n">
-        <v>5.735398772720959</v>
+        <v>1895.230148054891</v>
       </c>
       <c r="D129" t="n">
-        <v>234450485.8126971</v>
+        <v>228246618295.4416</v>
       </c>
       <c r="E129" t="n">
-        <v>12072109.71054304</v>
+        <v>6233921635.46938</v>
       </c>
     </row>
     <row r="130">
@@ -2642,16 +2642,16 @@
         <v>45055</v>
       </c>
       <c r="B130" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C130" t="n">
-        <v>5.734667116373509</v>
+        <v>1849.288629562528</v>
       </c>
       <c r="D130" t="n">
-        <v>234549492.8042675</v>
+        <v>222406833247.6045</v>
       </c>
       <c r="E130" t="n">
-        <v>8445492.056392189</v>
+        <v>11496171817.8335</v>
       </c>
     </row>
     <row r="131">
@@ -2659,16 +2659,16 @@
         <v>45056</v>
       </c>
       <c r="B131" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C131" t="n">
-        <v>5.613870755829392</v>
+        <v>1846.064264023148</v>
       </c>
       <c r="D131" t="n">
-        <v>229865023.0305036</v>
+        <v>222246427487.2296</v>
       </c>
       <c r="E131" t="n">
-        <v>9827133.558193048</v>
+        <v>6373057170.18455</v>
       </c>
     </row>
     <row r="132">
@@ -2676,16 +2676,16 @@
         <v>45057</v>
       </c>
       <c r="B132" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C132" t="n">
-        <v>5.50570986216366</v>
+        <v>1842.865558834664</v>
       </c>
       <c r="D132" t="n">
-        <v>225062017.4909179</v>
+        <v>221632027136.726</v>
       </c>
       <c r="E132" t="n">
-        <v>5754728.842277005</v>
+        <v>10471130832.93585</v>
       </c>
     </row>
     <row r="133">
@@ -2693,16 +2693,16 @@
         <v>45058</v>
       </c>
       <c r="B133" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C133" t="n">
-        <v>5.548529830921952</v>
+        <v>1798.071945526263</v>
       </c>
       <c r="D133" t="n">
-        <v>227269909.3006576</v>
+        <v>216323022928.9258</v>
       </c>
       <c r="E133" t="n">
-        <v>2969260.874356112</v>
+        <v>9217787395.589426</v>
       </c>
     </row>
     <row r="134">
@@ -2710,16 +2710,16 @@
         <v>45059</v>
       </c>
       <c r="B134" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C134" t="n">
-        <v>5.495329930080742</v>
+        <v>1808.694999901569</v>
       </c>
       <c r="D134" t="n">
-        <v>226047307.8604075</v>
+        <v>217659652941.8761</v>
       </c>
       <c r="E134" t="n">
-        <v>2228104.24632756</v>
+        <v>10530874714.29914</v>
       </c>
     </row>
     <row r="135">
@@ -2727,16 +2727,16 @@
         <v>45060</v>
       </c>
       <c r="B135" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C135" t="n">
-        <v>5.548586174948639</v>
+        <v>1797.19947013765</v>
       </c>
       <c r="D135" t="n">
-        <v>228065159.1634643</v>
+        <v>216032102439.7302</v>
       </c>
       <c r="E135" t="n">
-        <v>3811657.260327255</v>
+        <v>5150212384.025403</v>
       </c>
     </row>
     <row r="136">
@@ -2744,16 +2744,16 @@
         <v>45061</v>
       </c>
       <c r="B136" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C136" t="n">
-        <v>5.566690825620341</v>
+        <v>1799.008658615005</v>
       </c>
       <c r="D136" t="n">
-        <v>228616986.564254</v>
+        <v>216439514891.8453</v>
       </c>
       <c r="E136" t="n">
-        <v>2748769.828723324</v>
+        <v>4914907456.467633</v>
       </c>
     </row>
     <row r="137">
@@ -2761,16 +2761,16 @@
         <v>45062</v>
       </c>
       <c r="B137" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C137" t="n">
-        <v>5.496203816359802</v>
+        <v>1820.044759540719</v>
       </c>
       <c r="D137" t="n">
-        <v>225850945.8150719</v>
+        <v>218513683684.0507</v>
       </c>
       <c r="E137" t="n">
-        <v>2941484.15238882</v>
+        <v>7655256291.360313</v>
       </c>
     </row>
     <row r="138">
@@ -2778,16 +2778,16 @@
         <v>45063</v>
       </c>
       <c r="B138" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C138" t="n">
-        <v>5.565346910926984</v>
+        <v>1823.663018347519</v>
       </c>
       <c r="D138" t="n">
-        <v>228420649.7325549</v>
+        <v>219562064257.9877</v>
       </c>
       <c r="E138" t="n">
-        <v>3050529.652839505</v>
+        <v>6283428506.771688</v>
       </c>
     </row>
     <row r="139">
@@ -2795,16 +2795,16 @@
         <v>45064</v>
       </c>
       <c r="B139" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C139" t="n">
-        <v>5.49805151960381</v>
+        <v>1821.050634709663</v>
       </c>
       <c r="D139" t="n">
-        <v>226501007.3587001</v>
+        <v>219124262711.374</v>
       </c>
       <c r="E139" t="n">
-        <v>3450706.529144899</v>
+        <v>6647945218.37179</v>
       </c>
     </row>
     <row r="140">
@@ -2812,16 +2812,16 @@
         <v>45065</v>
       </c>
       <c r="B140" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C140" t="n">
-        <v>5.467942617870442</v>
+        <v>1802.390955483449</v>
       </c>
       <c r="D140" t="n">
-        <v>224905729.8948302</v>
+        <v>217078808863.7798</v>
       </c>
       <c r="E140" t="n">
-        <v>2784246.562209869</v>
+        <v>6170212643.307527</v>
       </c>
     </row>
     <row r="141">
@@ -2829,16 +2829,16 @@
         <v>45066</v>
       </c>
       <c r="B141" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C141" t="n">
-        <v>5.342225278946372</v>
+        <v>1812.131703560585</v>
       </c>
       <c r="D141" t="n">
-        <v>219574942.2205098</v>
+        <v>218083824882.0496</v>
       </c>
       <c r="E141" t="n">
-        <v>3191087.537625031</v>
+        <v>5092669091.509588</v>
       </c>
     </row>
     <row r="142">
@@ -2846,16 +2846,16 @@
         <v>45067</v>
       </c>
       <c r="B142" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C142" t="n">
-        <v>5.371228950612197</v>
+        <v>1818.969529503585</v>
       </c>
       <c r="D142" t="n">
-        <v>221105352.2065977</v>
+        <v>218770214155.4801</v>
       </c>
       <c r="E142" t="n">
-        <v>2590755.097513135</v>
+        <v>3117917206.10603</v>
       </c>
     </row>
     <row r="143">
@@ -2863,16 +2863,16 @@
         <v>45068</v>
       </c>
       <c r="B143" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C143" t="n">
-        <v>5.38529250580239</v>
+        <v>1804.92906710728</v>
       </c>
       <c r="D143" t="n">
-        <v>221799994.3693085</v>
+        <v>217302257173.6874</v>
       </c>
       <c r="E143" t="n">
-        <v>2564241.866529394</v>
+        <v>3835867355.217711</v>
       </c>
     </row>
     <row r="144">
@@ -2880,16 +2880,16 @@
         <v>45069</v>
       </c>
       <c r="B144" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C144" t="n">
-        <v>5.478609949831124</v>
+        <v>1818.401464498085</v>
       </c>
       <c r="D144" t="n">
-        <v>225423585.2004959</v>
+        <v>218746186925.5668</v>
       </c>
       <c r="E144" t="n">
-        <v>2780602.455942444</v>
+        <v>5183573151.892912</v>
       </c>
     </row>
     <row r="145">
@@ -2897,16 +2897,16 @@
         <v>45070</v>
       </c>
       <c r="B145" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C145" t="n">
-        <v>5.294945264646726</v>
+        <v>1854.193118273178</v>
       </c>
       <c r="D145" t="n">
-        <v>218249619.0033218</v>
+        <v>222906967413.9726</v>
       </c>
       <c r="E145" t="n">
-        <v>2758726.911382264</v>
+        <v>7537701078.994168</v>
       </c>
     </row>
     <row r="146">
@@ -2914,16 +2914,16 @@
         <v>45071</v>
       </c>
       <c r="B146" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C146" t="n">
-        <v>5.15498959975382</v>
+        <v>1800.736010305837</v>
       </c>
       <c r="D146" t="n">
-        <v>212491917.614959</v>
+        <v>216837950430.067</v>
       </c>
       <c r="E146" t="n">
-        <v>3177901.867683638</v>
+        <v>8000139188.961748</v>
       </c>
     </row>
     <row r="147">
@@ -2931,16 +2931,16 @@
         <v>45072</v>
       </c>
       <c r="B147" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C147" t="n">
-        <v>5.185578232143622</v>
+        <v>1805.805760405694</v>
       </c>
       <c r="D147" t="n">
-        <v>213986593.9355356</v>
+        <v>217194191610.3175</v>
       </c>
       <c r="E147" t="n">
-        <v>2234235.455684478</v>
+        <v>7459269403.375004</v>
       </c>
     </row>
     <row r="148">
@@ -2948,16 +2948,16 @@
         <v>45073</v>
       </c>
       <c r="B148" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C148" t="n">
-        <v>5.217261613274497</v>
+        <v>1828.956536619728</v>
       </c>
       <c r="D148" t="n">
-        <v>215465125.4529064</v>
+        <v>219969209232.7905</v>
       </c>
       <c r="E148" t="n">
-        <v>1857397.715703446</v>
+        <v>6245753617.103617</v>
       </c>
     </row>
     <row r="149">
@@ -2965,16 +2965,16 @@
         <v>45074</v>
       </c>
       <c r="B149" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C149" t="n">
-        <v>5.36666111464625</v>
+        <v>1830.306651316898</v>
       </c>
       <c r="D149" t="n">
-        <v>221783456.8197581</v>
+        <v>220035586188.3539</v>
       </c>
       <c r="E149" t="n">
-        <v>2649323.216196859</v>
+        <v>4068177989.627464</v>
       </c>
     </row>
     <row r="150">
@@ -2982,16 +2982,16 @@
         <v>45075</v>
       </c>
       <c r="B150" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C150" t="n">
-        <v>5.364147038974299</v>
+        <v>1913.816249316578</v>
       </c>
       <c r="D150" t="n">
-        <v>221547125.492898</v>
+        <v>230041639357.4828</v>
       </c>
       <c r="E150" t="n">
-        <v>3827086.693504286</v>
+        <v>7227287064.56947</v>
       </c>
     </row>
     <row r="151">
@@ -2999,16 +2999,16 @@
         <v>45076</v>
       </c>
       <c r="B151" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C151" t="n">
-        <v>5.360023977267692</v>
+        <v>1893.714274089704</v>
       </c>
       <c r="D151" t="n">
-        <v>221726379.3366231</v>
+        <v>227805314887.0995</v>
       </c>
       <c r="E151" t="n">
-        <v>2402842.712931514</v>
+        <v>6762040908.702834</v>
       </c>
     </row>
     <row r="152">
@@ -3016,16 +3016,16 @@
         <v>45077</v>
       </c>
       <c r="B152" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C152" t="n">
-        <v>5.215645605634681</v>
+        <v>1901.078310164527</v>
       </c>
       <c r="D152" t="n">
-        <v>215599403.8997818</v>
+        <v>228588229006.9005</v>
       </c>
       <c r="E152" t="n">
-        <v>2970390.094436291</v>
+        <v>6019457141.148654</v>
       </c>
     </row>
     <row r="153">
@@ -3033,16 +3033,16 @@
         <v>45078</v>
       </c>
       <c r="B153" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C153" t="n">
-        <v>5.256944401868377</v>
+        <v>1874.694885027078</v>
       </c>
       <c r="D153" t="n">
-        <v>217421206.4773878</v>
+        <v>225483513769.4682</v>
       </c>
       <c r="E153" t="n">
-        <v>2292276.945087925</v>
+        <v>5930556981.74496</v>
       </c>
     </row>
     <row r="154">
@@ -3050,16 +3050,16 @@
         <v>45079</v>
       </c>
       <c r="B154" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C154" t="n">
-        <v>5.383499820124367</v>
+        <v>1861.725386947619</v>
       </c>
       <c r="D154" t="n">
-        <v>222688184.1444947</v>
+        <v>223850958023.0443</v>
       </c>
       <c r="E154" t="n">
-        <v>2414335.481862423</v>
+        <v>6237923582.653606</v>
       </c>
     </row>
     <row r="155">
@@ -3067,16 +3067,16 @@
         <v>45080</v>
       </c>
       <c r="B155" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C155" t="n">
-        <v>5.204529852613117</v>
+        <v>1907.212321851007</v>
       </c>
       <c r="D155" t="n">
-        <v>215445865.6377138</v>
+        <v>229335461597.8791</v>
       </c>
       <c r="E155" t="n">
-        <v>2010790.656442622</v>
+        <v>6910486182.970303</v>
       </c>
     </row>
     <row r="156">
@@ -3084,16 +3084,16 @@
         <v>45081</v>
       </c>
       <c r="B156" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C156" t="n">
-        <v>5.257227936598536</v>
+        <v>1892.078176464758</v>
       </c>
       <c r="D156" t="n">
-        <v>217737006.9100954</v>
+        <v>227515751048.9767</v>
       </c>
       <c r="E156" t="n">
-        <v>2125863.150497312</v>
+        <v>3798117031.943575</v>
       </c>
     </row>
     <row r="157">
@@ -3101,16 +3101,16 @@
         <v>45082</v>
       </c>
       <c r="B157" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C157" t="n">
-        <v>4.941789296216165</v>
+        <v>1893.178280382087</v>
       </c>
       <c r="D157" t="n">
-        <v>204771063.315017</v>
+        <v>227418753400.9453</v>
       </c>
       <c r="E157" t="n">
-        <v>4636023.304120066</v>
+        <v>4274226592.398274</v>
       </c>
     </row>
     <row r="158">
@@ -3118,16 +3118,16 @@
         <v>45083</v>
       </c>
       <c r="B158" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C158" t="n">
-        <v>5.078174530566044</v>
+        <v>1813.6816549004</v>
       </c>
       <c r="D158" t="n">
-        <v>210306830.4697849</v>
+        <v>218224817446.1936</v>
       </c>
       <c r="E158" t="n">
-        <v>2587456.603527867</v>
+        <v>10887461193.43077</v>
       </c>
     </row>
     <row r="159">
@@ -3135,16 +3135,16 @@
         <v>45084</v>
       </c>
       <c r="B159" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C159" t="n">
-        <v>4.931176021743806</v>
+        <v>1883.242584625582</v>
       </c>
       <c r="D159" t="n">
-        <v>204300136.6245005</v>
+        <v>226225955928.725</v>
       </c>
       <c r="E159" t="n">
-        <v>3587337.089913819</v>
+        <v>9540379707.014326</v>
       </c>
     </row>
     <row r="160">
@@ -3152,16 +3152,16 @@
         <v>45085</v>
       </c>
       <c r="B160" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C160" t="n">
-        <v>4.933525329058218</v>
+        <v>1832.320402503454</v>
       </c>
       <c r="D160" t="n">
-        <v>204796529.8890513</v>
+        <v>220285044251.9128</v>
       </c>
       <c r="E160" t="n">
-        <v>2264561.631983673</v>
+        <v>8474108659.099132</v>
       </c>
     </row>
     <row r="161">
@@ -3169,16 +3169,16 @@
         <v>45086</v>
       </c>
       <c r="B161" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C161" t="n">
-        <v>4.884116883584625</v>
+        <v>1846.030001782057</v>
       </c>
       <c r="D161" t="n">
-        <v>202610951.8155374</v>
+        <v>222012641423.2545</v>
       </c>
       <c r="E161" t="n">
-        <v>2876981.81138987</v>
+        <v>4854817113.536453</v>
       </c>
     </row>
     <row r="162">
@@ -3186,16 +3186,16 @@
         <v>45087</v>
       </c>
       <c r="B162" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C162" t="n">
-        <v>4.603933301821398</v>
+        <v>1839.208012658193</v>
       </c>
       <c r="D162" t="n">
-        <v>191175833.6567698</v>
+        <v>221018802010.8545</v>
       </c>
       <c r="E162" t="n">
-        <v>10064931.69248629</v>
+        <v>5093666796.918479</v>
       </c>
     </row>
     <row r="163">
@@ -3203,16 +3203,16 @@
         <v>45088</v>
       </c>
       <c r="B163" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C163" t="n">
-        <v>4.458491795321306</v>
+        <v>1754.673228410636</v>
       </c>
       <c r="D163" t="n">
-        <v>185165628.8038222</v>
+        <v>210950148701.2072</v>
       </c>
       <c r="E163" t="n">
-        <v>3541561.01070291</v>
+        <v>41417850678.71391</v>
       </c>
     </row>
     <row r="164">
@@ -3220,16 +3220,16 @@
         <v>45089</v>
       </c>
       <c r="B164" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C164" t="n">
-        <v>4.477303380225521</v>
+        <v>1751.72459650425</v>
       </c>
       <c r="D164" t="n">
-        <v>186057270.9044695</v>
+        <v>210604043872.2481</v>
       </c>
       <c r="E164" t="n">
-        <v>3014385.106294883</v>
+        <v>5031836446.183817</v>
       </c>
     </row>
     <row r="165">
@@ -3237,16 +3237,16 @@
         <v>45090</v>
       </c>
       <c r="B165" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C165" t="n">
-        <v>4.400495055694409</v>
+        <v>1742.596052566616</v>
       </c>
       <c r="D165" t="n">
-        <v>182927838.6633825</v>
+        <v>209462687695.9398</v>
       </c>
       <c r="E165" t="n">
-        <v>2675182.121545033</v>
+        <v>6731496663.213711</v>
       </c>
     </row>
     <row r="166">
@@ -3254,16 +3254,16 @@
         <v>45091</v>
       </c>
       <c r="B166" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C166" t="n">
-        <v>4.259130033176471</v>
+        <v>1736.789437167462</v>
       </c>
       <c r="D166" t="n">
-        <v>177070402.5277421</v>
+        <v>208703993936.8153</v>
       </c>
       <c r="E166" t="n">
-        <v>2787218.567747585</v>
+        <v>6798862284.580931</v>
       </c>
     </row>
     <row r="167">
@@ -3271,16 +3271,16 @@
         <v>45092</v>
       </c>
       <c r="B167" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C167" t="n">
-        <v>4.254143564742189</v>
+        <v>1650.676667553546</v>
       </c>
       <c r="D167" t="n">
-        <v>176940110.358155</v>
+        <v>198559274296.6206</v>
       </c>
       <c r="E167" t="n">
-        <v>3752227.48197625</v>
+        <v>8025571357.471881</v>
       </c>
     </row>
     <row r="168">
@@ -3288,16 +3288,16 @@
         <v>45093</v>
       </c>
       <c r="B168" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C168" t="n">
-        <v>4.343153191804229</v>
+        <v>1664.977462394022</v>
       </c>
       <c r="D168" t="n">
-        <v>180700616.3410212</v>
+        <v>200099209933.7168</v>
       </c>
       <c r="E168" t="n">
-        <v>2223889.397961191</v>
+        <v>8283225649.876287</v>
       </c>
     </row>
     <row r="169">
@@ -3305,16 +3305,16 @@
         <v>45094</v>
       </c>
       <c r="B169" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C169" t="n">
-        <v>4.433507964305391</v>
+        <v>1716.377281092857</v>
       </c>
       <c r="D169" t="n">
-        <v>184434527.1559355</v>
+        <v>206321573355.8955</v>
       </c>
       <c r="E169" t="n">
-        <v>2115613.583638641</v>
+        <v>7008799576.154325</v>
       </c>
     </row>
     <row r="170">
@@ -3322,16 +3322,16 @@
         <v>45095</v>
       </c>
       <c r="B170" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C170" t="n">
-        <v>4.390437853425803</v>
+        <v>1726.372809734998</v>
       </c>
       <c r="D170" t="n">
-        <v>182470164.9654385</v>
+        <v>207595972780.2269</v>
       </c>
       <c r="E170" t="n">
-        <v>2164670.879933596</v>
+        <v>4859690685.481605</v>
       </c>
     </row>
     <row r="171">
@@ -3339,16 +3339,16 @@
         <v>45096</v>
       </c>
       <c r="B171" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C171" t="n">
-        <v>4.385147385185642</v>
+        <v>1719.273161506867</v>
       </c>
       <c r="D171" t="n">
-        <v>182557378.6486974</v>
+        <v>206730774198.4613</v>
       </c>
       <c r="E171" t="n">
-        <v>2040887.182493703</v>
+        <v>4084738737.028457</v>
       </c>
     </row>
     <row r="172">
@@ -3356,16 +3356,16 @@
         <v>45097</v>
       </c>
       <c r="B172" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C172" t="n">
-        <v>4.535611404626176</v>
+        <v>1734.793103442663</v>
       </c>
       <c r="D172" t="n">
-        <v>189502806.3706388</v>
+        <v>208507638780.8943</v>
       </c>
       <c r="E172" t="n">
-        <v>2295275.834275481</v>
+        <v>5770983890.906085</v>
       </c>
     </row>
     <row r="173">
@@ -3373,16 +3373,16 @@
         <v>45098</v>
       </c>
       <c r="B173" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C173" t="n">
-        <v>4.764312903609791</v>
+        <v>1790.190440731765</v>
       </c>
       <c r="D173" t="n">
-        <v>198639040.9889359</v>
+        <v>215060967094.1403</v>
       </c>
       <c r="E173" t="n">
-        <v>3147807.563116541</v>
+        <v>7900259127.350303</v>
       </c>
     </row>
     <row r="174">
@@ -3390,16 +3390,16 @@
         <v>45099</v>
       </c>
       <c r="B174" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C174" t="n">
-        <v>4.720661886366051</v>
+        <v>1892.899571916819</v>
       </c>
       <c r="D174" t="n">
-        <v>196238317.4014905</v>
+        <v>227581626984.1515</v>
       </c>
       <c r="E174" t="n">
-        <v>2457949.276116415</v>
+        <v>12294793429.60021</v>
       </c>
     </row>
     <row r="175">
@@ -3407,16 +3407,16 @@
         <v>45100</v>
       </c>
       <c r="B175" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C175" t="n">
-        <v>4.739416956439571</v>
+        <v>1874.177947016714</v>
       </c>
       <c r="D175" t="n">
-        <v>198540920.7099358</v>
+        <v>225381084937.8792</v>
       </c>
       <c r="E175" t="n">
-        <v>2598418.346490157</v>
+        <v>9842202528.707741</v>
       </c>
     </row>
     <row r="176">
@@ -3424,16 +3424,16 @@
         <v>45101</v>
       </c>
       <c r="B176" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C176" t="n">
-        <v>4.736144250326912</v>
+        <v>1891.345008021678</v>
       </c>
       <c r="D176" t="n">
-        <v>197627512.7334889</v>
+        <v>227419416441.5965</v>
       </c>
       <c r="E176" t="n">
-        <v>2249189.021426616</v>
+        <v>9303341351.325251</v>
       </c>
     </row>
     <row r="177">
@@ -3441,16 +3441,16 @@
         <v>45102</v>
       </c>
       <c r="B177" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C177" t="n">
-        <v>4.861574120802684</v>
+        <v>1875.059961928488</v>
       </c>
       <c r="D177" t="n">
-        <v>202948337.2697746</v>
+        <v>225448939889.3551</v>
       </c>
       <c r="E177" t="n">
-        <v>6205666.888157346</v>
+        <v>4889178964.702732</v>
       </c>
     </row>
     <row r="178">
@@ -3458,16 +3458,16 @@
         <v>45103</v>
       </c>
       <c r="B178" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C178" t="n">
-        <v>4.670979790592192</v>
+        <v>1899.147312104605</v>
       </c>
       <c r="D178" t="n">
-        <v>194771502.8114795</v>
+        <v>228332438014.1302</v>
       </c>
       <c r="E178" t="n">
-        <v>5473179.762472614</v>
+        <v>7363880089.050316</v>
       </c>
     </row>
     <row r="179">
@@ -3475,16 +3475,16 @@
         <v>45104</v>
       </c>
       <c r="B179" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C179" t="n">
-        <v>4.7875143471057</v>
+        <v>1859.802419642797</v>
       </c>
       <c r="D179" t="n">
-        <v>200452678.3169947</v>
+        <v>223061316934.5412</v>
       </c>
       <c r="E179" t="n">
-        <v>2652492.300948566</v>
+        <v>9893270861.839865</v>
       </c>
     </row>
     <row r="180">
@@ -3492,16 +3492,16 @@
         <v>45105</v>
       </c>
       <c r="B180" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C180" t="n">
-        <v>4.527078199847525</v>
+        <v>1890.012903783708</v>
       </c>
       <c r="D180" t="n">
-        <v>189157314.5009291</v>
+        <v>227143144300.6532</v>
       </c>
       <c r="E180" t="n">
-        <v>3111423.967025772</v>
+        <v>8806434878.376961</v>
       </c>
     </row>
     <row r="181">
@@ -3509,16 +3509,16 @@
         <v>45106</v>
       </c>
       <c r="B181" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C181" t="n">
-        <v>4.579037387095468</v>
+        <v>1828.458336400725</v>
       </c>
       <c r="D181" t="n">
-        <v>191466014.6204602</v>
+        <v>219923192180.6849</v>
       </c>
       <c r="E181" t="n">
-        <v>2412235.181158602</v>
+        <v>6821723542.735137</v>
       </c>
     </row>
     <row r="182">
@@ -3526,16 +3526,16 @@
         <v>45107</v>
       </c>
       <c r="B182" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C182" t="n">
-        <v>4.823335058835206</v>
+        <v>1853.445245874994</v>
       </c>
       <c r="D182" t="n">
-        <v>201695033.3499603</v>
+        <v>222892015037.6711</v>
       </c>
       <c r="E182" t="n">
-        <v>6313616.175886103</v>
+        <v>6609358548.632103</v>
       </c>
     </row>
     <row r="183">
@@ -3543,135 +3543,16 @@
         <v>45108</v>
       </c>
       <c r="B183" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C183" t="n">
-        <v>4.905518017506242</v>
+        <v>1934.045714261775</v>
       </c>
       <c r="D183" t="n">
-        <v>204707216.9821532</v>
+        <v>232417040695.4234</v>
       </c>
       <c r="E183" t="n">
-        <v>2458946.545226043</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="2" t="n">
-        <v>45109</v>
-      </c>
-      <c r="B184" t="n">
-        <v>7</v>
-      </c>
-      <c r="C184" t="n">
-        <v>4.904505666133654</v>
-      </c>
-      <c r="D184" t="n">
-        <v>205122338.2427768</v>
-      </c>
-      <c r="E184" t="n">
-        <v>2765371.323144797</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" s="2" t="n">
-        <v>45110</v>
-      </c>
-      <c r="B185" t="n">
-        <v>6</v>
-      </c>
-      <c r="C185" t="n">
-        <v>4.966507385014663</v>
-      </c>
-      <c r="D185" t="n">
-        <v>207648032.9476196</v>
-      </c>
-      <c r="E185" t="n">
-        <v>3658939.226958354</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" s="2" t="n">
-        <v>45111</v>
-      </c>
-      <c r="B186" t="n">
-        <v>5</v>
-      </c>
-      <c r="C186" t="n">
-        <v>4.838421597291229</v>
-      </c>
-      <c r="D186" t="n">
-        <v>203105542.9265649</v>
-      </c>
-      <c r="E186" t="n">
-        <v>4350471.560612216</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" s="2" t="n">
-        <v>45112</v>
-      </c>
-      <c r="B187" t="n">
-        <v>4</v>
-      </c>
-      <c r="C187" t="n">
-        <v>4.750384825937422</v>
-      </c>
-      <c r="D187" t="n">
-        <v>199215088.1268154</v>
-      </c>
-      <c r="E187" t="n">
-        <v>3422983.337052448</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" s="2" t="n">
-        <v>45113</v>
-      </c>
-      <c r="B188" t="n">
-        <v>3</v>
-      </c>
-      <c r="C188" t="n">
-        <v>4.584274121132915</v>
-      </c>
-      <c r="D188" t="n">
-        <v>192892514.7239836</v>
-      </c>
-      <c r="E188" t="n">
-        <v>4011919.860252854</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" s="2" t="n">
-        <v>45114</v>
-      </c>
-      <c r="B189" t="n">
-        <v>2</v>
-      </c>
-      <c r="C189" t="n">
-        <v>4.63067560943914</v>
-      </c>
-      <c r="D189" t="n">
-        <v>193662655.2218218</v>
-      </c>
-      <c r="E189" t="n">
-        <v>2609172.493560779</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" s="2" t="n">
-        <v>45115</v>
-      </c>
-      <c r="B190" t="n">
-        <v>1</v>
-      </c>
-      <c r="C190" t="n">
-        <v>4.591899766739614</v>
-      </c>
-      <c r="D190" t="n">
-        <v>192772957.9735725</v>
-      </c>
-      <c r="E190" t="n">
-        <v>2459909.234796377</v>
+        <v>11695335269.50953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>